<commit_message>
Updated data spreadsheets; added signature
</commit_message>
<xml_diff>
--- a/data/consultancy.xlsx
+++ b/data/consultancy.xlsx
@@ -1,26 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ueanorwich-my.sharepoint.com/personal/hpd08ucu_uea_ac_uk/Documents/CV/PL_CV/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="8_{9EFA0398-2594-4105-877E-470755A5DB01}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{80FADD69-8839-4798-8AD4-7BD218DFB468}"/>
+  <xr:revisionPtr revIDLastSave="89" documentId="8_{9EFA0398-2594-4105-877E-470755A5DB01}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC44CBEA-3040-4133-84F8-FFB086E0BCFA}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-4965" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="teaching" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>when</t>
   </si>
@@ -46,55 +57,52 @@
     <t>OCR</t>
   </si>
   <si>
-    <t>Resource Developer</t>
-  </si>
-  <si>
     <t>Programme Developer</t>
   </si>
   <si>
     <t>2020-present</t>
   </si>
   <si>
+    <t>Benchling</t>
+  </si>
+  <si>
+    <t>San Francisco</t>
+  </si>
+  <si>
+    <t>Oxford</t>
+  </si>
+  <si>
+    <t>Online</t>
+  </si>
+  <si>
+    <t>An Introduction to Population Genomics: covers and introduction to Linux OS, Python and R analysing NGS data and SNP calling</t>
+  </si>
+  <si>
+    <t>2016-present</t>
+  </si>
+  <si>
+    <t>Maths for Biology: Online workshops for secondary school teachers</t>
+  </si>
+  <si>
+    <t>The Scientific Method and Experimental Design (In prep) - part of the Oxford Biology Primers book series</t>
+  </si>
+  <si>
+    <t>Consultant and content developer</t>
+  </si>
+  <si>
+    <t>Consultancy and speaking</t>
+  </si>
+  <si>
+    <t>Content developer: https://www.benchling.com/educators/</t>
+  </si>
+  <si>
     <t>OUP</t>
   </si>
   <si>
-    <t>2016-2019</t>
-  </si>
-  <si>
-    <t>Editing &amp; Proofing</t>
-  </si>
-  <si>
     <t>Author</t>
   </si>
   <si>
-    <t>Maths Skills for A-level Biology</t>
-  </si>
-  <si>
-    <t>Benchling</t>
-  </si>
-  <si>
-    <t>Maths for Biology</t>
-  </si>
-  <si>
-    <t>Maths for Biology-Online</t>
-  </si>
-  <si>
-    <t>Introduction to Population Genomics</t>
-  </si>
-  <si>
-    <t>https://www.benchling.com/educators/</t>
-  </si>
-  <si>
-    <t>San Francisco</t>
-  </si>
-  <si>
-    <t>Oxford</t>
-  </si>
-  <si>
-    <t>Online</t>
-  </si>
-  <si>
-    <t>Populations, population growth and the species concept; Genetics and Evolution</t>
+    <t>Maths Skills for A-level Biology 2nd Edition: a practical handbook: https://amzn.to/3xjUUlN</t>
   </si>
 </sst>
 </file>
@@ -937,16 +945,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14.36328125" customWidth="1"/>
-    <col min="2" max="2" width="13.6328125" customWidth="1"/>
-    <col min="3" max="3" width="13.08984375" customWidth="1"/>
-    <col min="4" max="5" width="11.7265625" customWidth="1"/>
+    <col min="2" max="2" width="13.54296875" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="23.54296875" customWidth="1"/>
+    <col min="5" max="5" width="11.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -971,7 +980,7 @@
         <v>2019</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -980,15 +989,15 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>2016</v>
+      <c r="A3" t="s">
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -997,78 +1006,55 @@
         <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
         <v>22</v>
       </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>2018</v>
+      <c r="A6" t="s">
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" t="s">
-        <v>8</v>
-      </c>
       <c r="E7" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>